<commit_message>
update loai anh v2
</commit_message>
<xml_diff>
--- a/link.xlsx
+++ b/link.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Downloads\NhanDienVatThe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F83FE43-134D-49DB-88DF-5EEC11594C52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4439A156-5466-4C6C-A34D-B1ABDDDDDF78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1710" yWindow="2250" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,87 +31,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>link</t>
   </si>
   <si>
-    <t>https://shopee.vn/product/684900976/40268878921</t>
-  </si>
-  <si>
-    <t>https://shopee.vn/product/747298045/27828758849</t>
-  </si>
-  <si>
-    <t>https://shopee.vn/product/804021824/41171614363</t>
-  </si>
-  <si>
-    <t>https://shopee.vn/product/924360539/27571308838</t>
-  </si>
-  <si>
-    <t>https://shopee.vn/product/1528477619/40707052731</t>
-  </si>
-  <si>
-    <t>https://shopee.vn/product/1638404118/27692092259</t>
-  </si>
-  <si>
-    <t>https://shopee.vn/product/1378623975/25638056508</t>
-  </si>
-  <si>
-    <t>https://shopee.vn/product/1263784487/41274653739</t>
-  </si>
-  <si>
-    <t>https://shopee.vn/product/1608625285/41770468285</t>
-  </si>
-  <si>
-    <t>https://shopee.vn/product/1058429449/29160589976</t>
-  </si>
-  <si>
-    <t>https://shopee.vn/product/1058429449/26606463411</t>
-  </si>
-  <si>
-    <t>https://shopee.vn/product/1100423231/25875002171</t>
-  </si>
-  <si>
-    <t>https://shopee.vn/product/1326793022/27138730167</t>
-  </si>
-  <si>
-    <t>https://shopee.vn/product/445847087/23931362454</t>
-  </si>
-  <si>
-    <t>https://shopee.vn/product/1079744721/19494295476</t>
-  </si>
-  <si>
-    <t>https://shopee.vn/product/1128053573/41404025993</t>
-  </si>
-  <si>
-    <t>https://shopee.vn/product/969543159/25194082145</t>
-  </si>
-  <si>
-    <t>https://shopee.vn/product/1592501501/40268630998</t>
-  </si>
-  <si>
-    <t>https://shopee.vn/product/680623367/25573132212</t>
-  </si>
-  <si>
-    <t>https://shopee.vn/product/421677475/41115108228</t>
-  </si>
-  <si>
-    <t>https://shopee.vn/product/614226510/28066475960</t>
-  </si>
-  <si>
-    <t>https://shopee.vn/product/1484772661/26589479486</t>
-  </si>
-  <si>
-    <t>https://shopee.vn/product/361670377/41461483709</t>
-  </si>
-  <si>
-    <t>https://shopee.vn/product/1484771449/44361484016</t>
-  </si>
-  <si>
-    <t>https://shopee.vn/product/1027190654/26570183747</t>
-  </si>
-  <si>
-    <t>https://shopee.vn/product/1397391661/24438051490</t>
+    <t>combo 10 quần lót nữ su đúc cao cấp cạp cao tàn hình chữ GODDESS siêu đẹp | Shopee Việt Nam</t>
   </si>
 </sst>
 </file>
@@ -207,7 +132,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -249,6 +174,9 @@
           <etc:displayText val="2"/>
         </ext>
       </extLst>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -742,7 +670,7 @@
   <dimension ref="A1:Z977"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A27"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25"/>
@@ -754,15 +682,13 @@
     <col min="5" max="5" width="73.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:26" ht="15" thickBot="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:26">
-      <c r="A2" s="7" t="s">
-        <v>1</v>
-      </c>
+    <row r="2" spans="1:26" ht="15" thickBot="1">
+      <c r="A2" s="7"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="E2" s="2"/>
@@ -788,10 +714,8 @@
       <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
     </row>
-    <row r="3" spans="1:26">
-      <c r="A3" s="7" t="s">
-        <v>2</v>
-      </c>
+    <row r="3" spans="1:26" ht="15" thickBot="1">
+      <c r="A3" s="8"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="E3" s="2"/>
@@ -817,10 +741,8 @@
       <c r="Y3" s="2"/>
       <c r="Z3" s="2"/>
     </row>
-    <row r="4" spans="1:26">
-      <c r="A4" s="7" t="s">
-        <v>3</v>
-      </c>
+    <row r="4" spans="1:26" ht="15" thickBot="1">
+      <c r="A4" s="7"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="E4" s="2"/>
@@ -846,9 +768,9 @@
       <c r="Y4" s="2"/>
       <c r="Z4" s="2"/>
     </row>
-    <row r="5" spans="1:26">
-      <c r="A5" s="7" t="s">
-        <v>4</v>
+    <row r="5" spans="1:26" ht="15" thickBot="1">
+      <c r="A5" s="8" t="s">
+        <v>1</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -875,10 +797,8 @@
       <c r="Y5" s="2"/>
       <c r="Z5" s="2"/>
     </row>
-    <row r="6" spans="1:26">
-      <c r="A6" s="7" t="s">
-        <v>5</v>
-      </c>
+    <row r="6" spans="1:26" ht="15" thickBot="1">
+      <c r="A6" s="7"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="E6" s="2"/>
@@ -905,9 +825,7 @@
       <c r="Z6" s="2"/>
     </row>
     <row r="7" spans="1:26">
-      <c r="A7" s="7" t="s">
-        <v>6</v>
-      </c>
+      <c r="A7" s="7"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="E7" s="2"/>
@@ -934,9 +852,7 @@
       <c r="Z7" s="2"/>
     </row>
     <row r="8" spans="1:26">
-      <c r="A8" s="7" t="s">
-        <v>7</v>
-      </c>
+      <c r="A8" s="7"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="E8" s="2"/>
@@ -963,9 +879,7 @@
       <c r="Z8" s="2"/>
     </row>
     <row r="9" spans="1:26">
-      <c r="A9" s="7" t="s">
-        <v>8</v>
-      </c>
+      <c r="A9" s="7"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="E9" s="2"/>
@@ -992,9 +906,7 @@
       <c r="Z9" s="2"/>
     </row>
     <row r="10" spans="1:26">
-      <c r="A10" s="7" t="s">
-        <v>9</v>
-      </c>
+      <c r="A10" s="7"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="E10" s="2"/>
@@ -1021,9 +933,7 @@
       <c r="Z10" s="2"/>
     </row>
     <row r="11" spans="1:26">
-      <c r="A11" s="7" t="s">
-        <v>10</v>
-      </c>
+      <c r="A11" s="7"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="E11" s="2"/>
@@ -1050,9 +960,7 @@
       <c r="Z11" s="2"/>
     </row>
     <row r="12" spans="1:26">
-      <c r="A12" s="7" t="s">
-        <v>11</v>
-      </c>
+      <c r="A12" s="7"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="E12" s="2"/>
@@ -1079,9 +987,7 @@
       <c r="Z12" s="2"/>
     </row>
     <row r="13" spans="1:26">
-      <c r="A13" s="7" t="s">
-        <v>12</v>
-      </c>
+      <c r="A13" s="7"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="E13" s="2"/>
@@ -1108,9 +1014,7 @@
       <c r="Z13" s="2"/>
     </row>
     <row r="14" spans="1:26">
-      <c r="A14" s="7" t="s">
-        <v>13</v>
-      </c>
+      <c r="A14" s="7"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="E14" s="2"/>
@@ -1137,9 +1041,7 @@
       <c r="Z14" s="2"/>
     </row>
     <row r="15" spans="1:26">
-      <c r="A15" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="A15" s="7"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="E15" s="2"/>
@@ -1166,9 +1068,7 @@
       <c r="Z15" s="2"/>
     </row>
     <row r="16" spans="1:26">
-      <c r="A16" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="E16" s="2"/>
@@ -1195,9 +1095,7 @@
       <c r="Z16" s="2"/>
     </row>
     <row r="17" spans="1:26">
-      <c r="A17" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="E17" s="2"/>
@@ -1224,9 +1122,7 @@
       <c r="Z17" s="2"/>
     </row>
     <row r="18" spans="1:26">
-      <c r="A18" s="1" t="s">
-        <v>17</v>
-      </c>
+      <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="E18" s="2"/>
@@ -1253,9 +1149,7 @@
       <c r="Z18" s="2"/>
     </row>
     <row r="19" spans="1:26">
-      <c r="A19" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="A19" s="1"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="E19" s="2"/>
@@ -1282,9 +1176,7 @@
       <c r="Z19" s="2"/>
     </row>
     <row r="20" spans="1:26">
-      <c r="A20" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="A20" s="1"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="E20" s="2"/>
@@ -1311,9 +1203,7 @@
       <c r="Z20" s="2"/>
     </row>
     <row r="21" spans="1:26">
-      <c r="A21" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="E21" s="2"/>
@@ -1340,9 +1230,7 @@
       <c r="Z21" s="2"/>
     </row>
     <row r="22" spans="1:26">
-      <c r="A22" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="E22" s="2"/>
@@ -1369,9 +1257,7 @@
       <c r="Z22" s="2"/>
     </row>
     <row r="23" spans="1:26">
-      <c r="A23" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="A23" s="1"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="E23" s="2"/>
@@ -1398,9 +1284,7 @@
       <c r="Z23" s="2"/>
     </row>
     <row r="24" spans="1:26">
-      <c r="A24" s="1" t="s">
-        <v>23</v>
-      </c>
+      <c r="A24" s="1"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="E24" s="2"/>
@@ -1427,9 +1311,7 @@
       <c r="Z24" s="2"/>
     </row>
     <row r="25" spans="1:26">
-      <c r="A25" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="A25" s="1"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="E25" s="2"/>
@@ -1456,9 +1338,7 @@
       <c r="Z25" s="2"/>
     </row>
     <row r="26" spans="1:26">
-      <c r="A26" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="A26" s="1"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="E26" s="2"/>
@@ -1485,9 +1365,7 @@
       <c r="Z26" s="2"/>
     </row>
     <row r="27" spans="1:26">
-      <c r="A27" s="1" t="s">
-        <v>26</v>
-      </c>
+      <c r="A27" s="1"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="E27" s="2"/>
@@ -27546,6 +27424,9 @@
       <c r="Z977" s="2"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A5" r:id="rId1" display="https://shopee.vn/combo-10-qu%E1%BA%A7n-l%C3%B3t-n%E1%BB%AF-su-%C4%91%C3%BAc-cao-c%E1%BA%A5p-c%E1%BA%A1p-cao-t%C3%A0n-h%C3%ACnh-ch%E1%BB%AF-GODDESS-si%C3%AAu-%C4%91%E1%BA%B9p-i.237396802.22956820818?extraParams=%7B%22display_model_id%22%3A245036196414%2C%22model_selection_logic%22%3A3%7D&amp;sp_atk=3c207934-60e7-4630-80a1-25caa0819eb0&amp;xptdk=3c207934-60e7-4630-80a1-25caa0819eb0" xr:uid="{0F6B9278-DD57-4C03-84C3-D26227B5201B}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>

</xml_diff>

<commit_message>
update loai anh v3
</commit_message>
<xml_diff>
--- a/link.xlsx
+++ b/link.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Downloads\NhanDienVatThe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4439A156-5466-4C6C-A34D-B1ABDDDDDF78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C068019-42A5-42B0-821B-5FB97EB3934D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1710" yWindow="2250" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,19 +31,22 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>link</t>
   </si>
   <si>
-    <t>combo 10 quần lót nữ su đúc cao cấp cạp cao tàn hình chữ GODDESS siêu đẹp | Shopee Việt Nam</t>
+    <t>https://shopee.vn/%C3%81o-L%C3%B3t-N%E1%BB%AF-%C3%81o-Ng%E1%BB%B1c-Hai-Khuy-C%C3%A0i-Tr%C6%B0%E1%BB%9Bc-%C3%81o-L%C3%B3t-Ren-N%E1%BB%AF-C%C3%B3-Th%E1%BB%83-Th%C3%A1o-D%C3%A2y-Ch%E1%BB%91ng-T%E1%BB%A5t-Quy%E1%BA%BFn-R%C5%A9-Cho-N%E1%BB%AF-Avalingerie-AL0041-i.406988686.24371376553?extraParams=%7B%22display_model_id%22%3A217401149751%2C%22model_selection_logic%22%3A3%7D&amp;sp_atk=6e861c42-5a06-4b5d-95e0-88d52353476e&amp;xptdk=6e861c42-5a06-4b5d-95e0-88d52353476e</t>
+  </si>
+  <si>
+    <t>https://s.shopee.vn/12HJWTN2s</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -78,6 +81,11 @@
       <name val="Arial"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF65686C"/>
+      <name val="Inherit"/>
     </font>
   </fonts>
   <fills count="4">
@@ -132,7 +140,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -177,6 +185,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -670,12 +684,12 @@
   <dimension ref="A1:Z977"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="39.625" customWidth="1"/>
+    <col min="1" max="1" width="63.75" customWidth="1"/>
     <col min="2" max="2" width="5.75" customWidth="1"/>
     <col min="3" max="3" width="5" customWidth="1"/>
     <col min="4" max="4" width="45.625" customWidth="1"/>
@@ -687,8 +701,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="15" thickBot="1">
-      <c r="A2" s="7"/>
+    <row r="2" spans="1:26" ht="153.75" customHeight="1" thickBot="1">
+      <c r="A2" s="9" t="s">
+        <v>1</v>
+      </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="E2" s="2"/>
@@ -715,7 +731,9 @@
       <c r="Z2" s="2"/>
     </row>
     <row r="3" spans="1:26" ht="15" thickBot="1">
-      <c r="A3" s="8"/>
+      <c r="A3" s="8" t="s">
+        <v>2</v>
+      </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="E3" s="2"/>
@@ -742,7 +760,7 @@
       <c r="Z3" s="2"/>
     </row>
     <row r="4" spans="1:26" ht="15" thickBot="1">
-      <c r="A4" s="7"/>
+      <c r="A4" s="10"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="E4" s="2"/>
@@ -769,9 +787,7 @@
       <c r="Z4" s="2"/>
     </row>
     <row r="5" spans="1:26" ht="15" thickBot="1">
-      <c r="A5" s="8" t="s">
-        <v>1</v>
-      </c>
+      <c r="A5" s="9"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="E5" s="2"/>
@@ -798,7 +814,7 @@
       <c r="Z5" s="2"/>
     </row>
     <row r="6" spans="1:26" ht="15" thickBot="1">
-      <c r="A6" s="7"/>
+      <c r="A6" s="9"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="E6" s="2"/>
@@ -824,8 +840,7 @@
       <c r="Y6" s="2"/>
       <c r="Z6" s="2"/>
     </row>
-    <row r="7" spans="1:26">
-      <c r="A7" s="7"/>
+    <row r="7" spans="1:26" ht="15" thickBot="1">
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="E7" s="2"/>
@@ -851,7 +866,7 @@
       <c r="Y7" s="2"/>
       <c r="Z7" s="2"/>
     </row>
-    <row r="8" spans="1:26">
+    <row r="8" spans="1:26" ht="15" thickBot="1">
       <c r="A8" s="7"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -878,7 +893,7 @@
       <c r="Y8" s="2"/>
       <c r="Z8" s="2"/>
     </row>
-    <row r="9" spans="1:26">
+    <row r="9" spans="1:26" ht="15" thickBot="1">
       <c r="A9" s="7"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -27425,9 +27440,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A5" r:id="rId1" display="https://shopee.vn/combo-10-qu%E1%BA%A7n-l%C3%B3t-n%E1%BB%AF-su-%C4%91%C3%BAc-cao-c%E1%BA%A5p-c%E1%BA%A1p-cao-t%C3%A0n-h%C3%ACnh-ch%E1%BB%AF-GODDESS-si%C3%AAu-%C4%91%E1%BA%B9p-i.237396802.22956820818?extraParams=%7B%22display_model_id%22%3A245036196414%2C%22model_selection_logic%22%3A3%7D&amp;sp_atk=3c207934-60e7-4630-80a1-25caa0819eb0&amp;xptdk=3c207934-60e7-4630-80a1-25caa0819eb0" xr:uid="{0F6B9278-DD57-4C03-84C3-D26227B5201B}"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://shopee.vn/%C3%81o-L%C3%B3t-N%E1%BB%AF-%C3%81o-Ng%E1%BB%B1c-Hai-Khuy-C%C3%A0i-Tr%C6%B0%E1%BB%9Bc-%C3%81o-L%C3%B3t-Ren-N%E1%BB%AF-C%C3%B3-Th%E1%BB%83-Th%C3%A1o-D%C3%A2y-Ch%E1%BB%91ng-T%E1%BB%A5t-Quy%E1%BA%BFn-R%C5%A9-Cho-N%E1%BB%AF-Avalingerie-AL0041-i.406988686.24371376553?extraParams=%7B%22display_model_id%22%3A217401149751%2C%22model_selection_logic%22%3A3%7D&amp;sp_atk=6e861c42-5a06-4b5d-95e0-88d52353476e&amp;xptdk=6e861c42-5a06-4b5d-95e0-88d52353476e" xr:uid="{2DCC030A-D437-408C-A7D3-2892DD8B57B0}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{0B144FA4-7F6E-4D83-857A-EFD2FB8CEE15}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>